<commit_message>
[Add] libExcelToMysql.py [Add] flask server
</commit_message>
<xml_diff>
--- a/ExcelToMysqlConvertor/CreateTable.xlsx
+++ b/ExcelToMysqlConvertor/CreateTable.xlsx
@@ -8,25 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\PyCharm\PyTorch\couragesuper-ds\ExcelToMysqlConvertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DFC846-0358-4BF7-8CBC-8E3A92693EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E29D86-FD47-4D69-B201-EC0125DB05C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3B8308AB-14C0-4449-AAAA-ACF7A6B4983D}"/>
+    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{3B8308AB-14C0-4449-AAAA-ACF7A6B4983D}"/>
   </bookViews>
   <sheets>
     <sheet name="poem" sheetId="1" r:id="rId1"/>
     <sheet name="thanksdiary" sheetId="2" r:id="rId2"/>
+    <sheet name="praise" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="199">
   <si>
     <t>참 다행입니다.
 사랑이 진리이어서,
@@ -355,9 +362,6 @@
     <t>모든 것이 사랑</t>
   </si>
   <si>
-    <t>호모 Thankspian에 대한 것</t>
-  </si>
-  <si>
     <t>관계</t>
   </si>
   <si>
@@ -5367,6 +5371,309 @@
   </si>
   <si>
     <t>감사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>호모</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Thankspian</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>에</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>대한</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>것</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VideoID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>brief</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dance  like david dance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=g7cnJOiY2LI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예배 마다 오시는 성령을 법궤 삼아서, 찬양으로 준비하는 마음을 묵상하게 해준 영상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽임당한 그 어린양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lNOj5y5ydec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태국 선교가서 처음 몸춤의 은사를 받을 떄, 듣고 있었던 찬양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몸춤 은사를 받을 때 듣던 곡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽임당한 그 어린양(global version)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LpcvT7K6U3g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZFvgIjOv-rA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽임당한 그 어린양 (다국어버전)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>몸찬양의 끝을 어디로 잡아야 할지 영감을 준 곡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">이 아침에 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hujquv5T94w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교회에서 오후 예배를 마치고, 새벽예배를 기약할 때에 많이 불렀던 곡입니다.
+모든 것이 감사하다는 구절에서 감동을 얻어서 많이 눈물을 흘리곤 했습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송축해 내 영혼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GSVF99daDBg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>송축해 내 영혼(10,000 Reason)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=FWUMFtboTTI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>만번의 감사제사 제목의 영감</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시선</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-lkph0w6PSA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오후 찬양예배에서 몸찬양을 드린 이후에 많이 듣게되었습니다.
+나를 통하여, 하나님이 일하실 것이란 소망을 다시 뜨겁게 하고,
+소망하게 하는 곡입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쉐카이나 영광(스캇 브래너)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RHJoUXJohak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>태국 선교 갈 즈음에 접하게 된 찬양인데, 라이브로 만들어진 풍이 
+매우 강한 영감을 주는 곡입니다. 
+여러가지 추억이 있는 곡인데, 태국 단기 선교중에 땅밝기 중에, 
+링싯 대학의 중앙에서 비바람이 몰아칠때, 우비를 입고 이 찬양을 들으며
+춤을 춘 기억이 있습니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하나님꼐서 세상을 사랑하사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ArS5QqH5Po8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">성수성전 기도실에서, 들으며 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부르신 곳에서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qck_76359CQ</t>
+  </si>
+  <si>
+    <t>예배와 찬양의 싸움을 할 때에 들으며, 묵상하던 찬양</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왕되신 주꼐 감사하세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=p7v4rNVbRLM</t>
+  </si>
+  <si>
+    <t>하나님의 이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>나의 주 나의 하나님이여 주를 경배합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=IZMzkTTnsPQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하나님께 드리려고 준비한 것들이 아무 성관없이 다 끝나는 듯 할때. 내가 드린 믿음의 고백</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>varchar(1000)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>related</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>g7cnJOiY2LI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lNOj5y5ydec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LpcvT7K6U3g</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ZFvgIjOv-rA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hujquv5T94w</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GSVF99daDBg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FWUMFtboTTI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RHJoUXJohak</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ArS5QqH5Po8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qck_76359CQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>p7v4rNVbRLM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IZMzkTTnsPQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-lkph0w6PSA</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5374,7 +5681,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5449,16 +5756,48 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -5481,13 +5820,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5518,9 +5875,31 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5834,7 +6213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE21A85-4DE9-4537-98D2-5988A6E7E42A}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -6005,8 +6384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A2581D-664D-4238-AE70-994B8F0A6E1B}">
   <dimension ref="A1:F85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E76" sqref="E76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6093,7 +6472,7 @@
         <v>34</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>35</v>
@@ -6113,7 +6492,7 @@
         <v>36</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>37</v>
@@ -6133,7 +6512,7 @@
         <v>38</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>39</v>
@@ -6153,7 +6532,7 @@
         <v>40</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8">
@@ -6171,7 +6550,7 @@
         <v>41</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>35</v>
@@ -6211,7 +6590,7 @@
         <v>44</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>45</v>
@@ -6231,7 +6610,7 @@
         <v>46</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>47</v>
@@ -6251,7 +6630,7 @@
         <v>48</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>47</v>
@@ -6271,7 +6650,7 @@
         <v>49</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>37</v>
@@ -6311,7 +6690,7 @@
         <v>51</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>47</v>
@@ -6331,7 +6710,7 @@
         <v>46</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>46</v>
@@ -6348,10 +6727,10 @@
         <v>20191204</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>52</v>
+        <v>115</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>141</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>46</v>
@@ -6368,13 +6747,13 @@
         <v>20191204</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -6388,13 +6767,13 @@
         <v>20191204</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -6408,13 +6787,13 @@
         <v>20191204</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -6428,10 +6807,10 @@
         <v>20191204</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>35</v>
@@ -6448,10 +6827,10 @@
         <v>20191204</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>37</v>
@@ -6468,13 +6847,13 @@
         <v>20191204</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -6488,13 +6867,13 @@
         <v>20191209</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>58</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -6508,10 +6887,10 @@
         <v>20191209</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>37</v>
@@ -6528,10 +6907,10 @@
         <v>20191209</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27">
@@ -6546,10 +6925,10 @@
         <v>20191209</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>45</v>
@@ -6566,10 +6945,10 @@
         <v>20191209</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>45</v>
@@ -6586,10 +6965,10 @@
         <v>20191209</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>45</v>
@@ -6606,13 +6985,13 @@
         <v>20191209</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -6626,13 +7005,13 @@
         <v>20191209</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -6646,10 +7025,10 @@
         <v>20191209</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>35</v>
@@ -6666,10 +7045,10 @@
         <v>20191209</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>47</v>
@@ -6686,10 +7065,10 @@
         <v>20191209</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>47</v>
@@ -6706,10 +7085,10 @@
         <v>20191210</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>35</v>
@@ -6726,10 +7105,10 @@
         <v>20191210</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>35</v>
@@ -6746,10 +7125,10 @@
         <v>20191210</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>47</v>
@@ -6766,10 +7145,10 @@
         <v>20191210</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>47</v>
@@ -6786,10 +7165,10 @@
         <v>20191210</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>47</v>
@@ -6806,10 +7185,10 @@
         <v>20191210</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>35</v>
@@ -6824,10 +7203,10 @@
       </c>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>35</v>
@@ -6844,10 +7223,10 @@
         <v>20191210</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>35</v>
@@ -6864,10 +7243,10 @@
         <v>20191210</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>45</v>
@@ -6884,13 +7263,13 @@
         <v>20191210</v>
       </c>
       <c r="C45" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>141</v>
-      </c>
       <c r="E45" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -6904,10 +7283,10 @@
         <v>20200410</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>45</v>
@@ -6924,13 +7303,13 @@
         <v>20200417</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -6944,10 +7323,10 @@
         <v>20200417</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48">
@@ -6962,10 +7341,10 @@
         <v>20200417</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49">
@@ -6980,10 +7359,10 @@
         <v>20200417</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50">
@@ -6998,10 +7377,10 @@
         <v>20200417</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51">
@@ -7016,13 +7395,13 @@
         <v>20200417</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -7036,13 +7415,13 @@
         <v>20200420</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -7056,13 +7435,13 @@
         <v>20200420</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -7076,13 +7455,13 @@
         <v>20200420</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -7096,13 +7475,13 @@
         <v>20200420</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -7116,10 +7495,10 @@
         <v>20200421</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E57" s="5" t="s">
         <v>35</v>
@@ -7136,7 +7515,7 @@
         <v>20200508</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>35</v>
@@ -7156,13 +7535,13 @@
         <v>20200508</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -7176,13 +7555,13 @@
         <v>20200508</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="E60" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="F60">
         <v>5</v>
@@ -7196,13 +7575,13 @@
         <v>20200508</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -7216,13 +7595,13 @@
         <v>20200508</v>
       </c>
       <c r="C62" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="F62">
         <v>10</v>
@@ -7237,7 +7616,7 @@
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E63" s="5"/>
       <c r="F63">
@@ -7252,13 +7631,13 @@
         <v>20200511</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F64">
         <v>5</v>
@@ -7272,13 +7651,13 @@
         <v>20200512</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="F65">
         <v>5</v>
@@ -7292,13 +7671,13 @@
         <v>20200512</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -7312,13 +7691,13 @@
         <v>20200512</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -7332,13 +7711,13 @@
         <v>20200513</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -7352,10 +7731,10 @@
         <v>20200513</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E69" s="5" t="s">
         <v>35</v>
@@ -7372,13 +7751,13 @@
         <v>20200522</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F70">
         <v>10</v>
@@ -7392,13 +7771,13 @@
         <v>20200527</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -7412,13 +7791,13 @@
         <v>20200601</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F72">
         <v>10</v>
@@ -7432,13 +7811,13 @@
         <v>20200601</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -7452,13 +7831,13 @@
         <v>20200602</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -7472,13 +7851,13 @@
         <v>20200603</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -7492,13 +7871,13 @@
         <v>20200604</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -7512,13 +7891,13 @@
         <v>20200605</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -7532,13 +7911,13 @@
         <v>20200606</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F78">
         <v>5</v>
@@ -7552,13 +7931,13 @@
         <v>20200606</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -7572,13 +7951,13 @@
         <v>20200607</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -7592,13 +7971,13 @@
         <v>20200608</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F81">
         <v>5</v>
@@ -7612,13 +7991,13 @@
         <v>20200608</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E82" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -7632,10 +8011,10 @@
         <v>20200608</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E83" s="5" t="s">
         <v>35</v>
@@ -7652,13 +8031,13 @@
         <v>20200609</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F84">
         <v>5</v>
@@ -7672,13 +8051,13 @@
         <v>20200609</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -7689,4 +8068,388 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B438DAE-6F36-41E3-B6E7-010F6023C9BC}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.75" style="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>2</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>4</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>5</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" ht="24" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>6</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>7</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>8</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A13" s="13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+      <c r="A14" s="13">
+        <v>10</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="13">
+        <v>11</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="13">
+        <v>12</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="13">
+        <v>13</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>14</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{726E30F9-A7BC-4B18-B3CE-3C2E756C4D62}"/>
+    <hyperlink ref="D8" r:id="rId2" xr:uid="{022DB076-2E91-4EA5-A55E-845117BDE037}"/>
+    <hyperlink ref="D9" r:id="rId3" xr:uid="{4A104A3B-43CE-4F2F-AEBE-D5B06F7DD87E}"/>
+    <hyperlink ref="D10" r:id="rId4" xr:uid="{E3515CC8-2440-4B36-B59F-0678466627DC}"/>
+    <hyperlink ref="D11" r:id="rId5" xr:uid="{A748D35F-35F8-4955-A175-C51252C9965A}"/>
+    <hyperlink ref="D12" r:id="rId6" xr:uid="{C4F137A2-0CA2-4C69-872A-81080BC8C680}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{A3E8E0CA-4BD4-4F4D-9A4B-900A056B41F0}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{EFB74637-34E3-4A63-894D-2DF869264FAA}"/>
+    <hyperlink ref="D7" r:id="rId9" xr:uid="{236562E9-D668-4EA2-9648-008B08B52BD2}"/>
+    <hyperlink ref="D15" r:id="rId10" xr:uid="{EDC8EC55-58B7-4706-92A6-1672B78E59FA}"/>
+    <hyperlink ref="D17" r:id="rId11" xr:uid="{62C24E9B-811F-40D1-B8CE-0DF3FC0F36AE}"/>
+    <hyperlink ref="D5" r:id="rId12" xr:uid="{C7CCEB96-EDDA-42E7-8B3A-6341F4D376DA}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{AF376E29-877B-4A14-BD5F-5E55BA20D6AA}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{C4F8BDCD-A499-4381-AB25-A8B2741C159E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[add] Common (Excel to Mysql), [add] UCC Crawler, [add] cvtFear init, [ENH] FLASK server, [ENH] SQLITE
</commit_message>
<xml_diff>
--- a/ExcelToMysqlConvertor/CreateTable.xlsx
+++ b/ExcelToMysqlConvertor/CreateTable.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\PyCharm\PyTorch\couragesuper-ds\ExcelToMysqlConvertor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E29D86-FD47-4D69-B201-EC0125DB05C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E7A91E0-678D-40CA-9412-B3E6432A2CEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1800" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{3B8308AB-14C0-4449-AAAA-ACF7A6B4983D}"/>
+    <workbookView xWindow="1650" yWindow="930" windowWidth="27000" windowHeight="14235" activeTab="3" xr2:uid="{3B8308AB-14C0-4449-AAAA-ACF7A6B4983D}"/>
   </bookViews>
   <sheets>
     <sheet name="poem" sheetId="1" r:id="rId1"/>
     <sheet name="thanksdiary" sheetId="2" r:id="rId2"/>
     <sheet name="praise" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="279">
   <si>
     <t>참 다행입니다.
 사랑이 진리이어서,
@@ -5674,6 +5675,251 @@
   </si>
   <si>
     <t>-lkph0w6PSA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출 1:21</t>
+  </si>
+  <si>
+    <t>다산을 주시는 분</t>
+  </si>
+  <si>
+    <t>출 20:20</t>
+  </si>
+  <si>
+    <t>죄를 짓지 않게 하시는 분</t>
+  </si>
+  <si>
+    <t>신 5:29</t>
+  </si>
+  <si>
+    <t>우리와 우리 자손에 대한 축복</t>
+  </si>
+  <si>
+    <t>잠 9:10-11</t>
+  </si>
+  <si>
+    <t>장수</t>
+  </si>
+  <si>
+    <t>잠 19:23</t>
+  </si>
+  <si>
+    <t>생명의 보전</t>
+  </si>
+  <si>
+    <t>전 8:12</t>
+  </si>
+  <si>
+    <t>성공</t>
+  </si>
+  <si>
+    <t>왕하 17:39</t>
+  </si>
+  <si>
+    <t>구원</t>
+  </si>
+  <si>
+    <t>느 5:9</t>
+  </si>
+  <si>
+    <t>존경</t>
+  </si>
+  <si>
+    <t>느 7:2</t>
+  </si>
+  <si>
+    <t>권위를 얻음</t>
+  </si>
+  <si>
+    <t>시 25:12</t>
+  </si>
+  <si>
+    <t>주의 가르침을 받음</t>
+  </si>
+  <si>
+    <t>시 111:5</t>
+  </si>
+  <si>
+    <t>양식을 공급받음</t>
+  </si>
+  <si>
+    <t>시 25:14</t>
+  </si>
+  <si>
+    <t>진리를 계시하심</t>
+  </si>
+  <si>
+    <t>시 31:19</t>
+  </si>
+  <si>
+    <t>풍성한 은혜</t>
+  </si>
+  <si>
+    <t>시 33:18</t>
+  </si>
+  <si>
+    <t>확실한 하나님의 보살피심</t>
+  </si>
+  <si>
+    <t>시 34:7</t>
+  </si>
+  <si>
+    <t>천사의 수호와 구원</t>
+  </si>
+  <si>
+    <t>시 34:9</t>
+  </si>
+  <si>
+    <t>모든 필요를 채우심</t>
+  </si>
+  <si>
+    <t>시 61:5</t>
+  </si>
+  <si>
+    <t>기업을 얻음</t>
+  </si>
+  <si>
+    <t>시 103:11</t>
+  </si>
+  <si>
+    <t>하나님의 인자하심을 얻음</t>
+  </si>
+  <si>
+    <t>시 103:13</t>
+  </si>
+  <si>
+    <t>긍휼하심을 얻음</t>
+  </si>
+  <si>
+    <t>하나님의 친밀함을 얻음</t>
+  </si>
+  <si>
+    <t>시 111:10</t>
+  </si>
+  <si>
+    <t>지혜</t>
+  </si>
+  <si>
+    <t>시 112:1</t>
+  </si>
+  <si>
+    <t>하나님의 축복</t>
+  </si>
+  <si>
+    <t>시 115:13~14</t>
+  </si>
+  <si>
+    <t>우리와 자녀에게 넘치도록 축복하심</t>
+  </si>
+  <si>
+    <t>시 128</t>
+  </si>
+  <si>
+    <t>가정을 축복하심</t>
+  </si>
+  <si>
+    <t>시 115:11</t>
+  </si>
+  <si>
+    <t>보호</t>
+  </si>
+  <si>
+    <t>시 119:63</t>
+  </si>
+  <si>
+    <t>하나님을 경외하는 자와 사귐</t>
+  </si>
+  <si>
+    <t>사 145:19</t>
+  </si>
+  <si>
+    <t>소원을 이룸</t>
+  </si>
+  <si>
+    <t>시 147:11</t>
+  </si>
+  <si>
+    <t>하나님이 우리를 기뻐하심</t>
+  </si>
+  <si>
+    <t>잠 3:7-8</t>
+  </si>
+  <si>
+    <t>치유와 회복</t>
+  </si>
+  <si>
+    <t>잠 14:26</t>
+  </si>
+  <si>
+    <t>하나님을 신뢰함 , 피난처 되심</t>
+  </si>
+  <si>
+    <t>말 3:16</t>
+  </si>
+  <si>
+    <t>하나님의 기념책에 기록됨</t>
+  </si>
+  <si>
+    <t>만족</t>
+  </si>
+  <si>
+    <t>잠 22:4</t>
+  </si>
+  <si>
+    <t>재물과 영광과 생명</t>
+  </si>
+  <si>
+    <t>잠 31:30</t>
+  </si>
+  <si>
+    <t>존귀한 여인</t>
+  </si>
+  <si>
+    <t>전 7:18</t>
+  </si>
+  <si>
+    <t>렘 32:40</t>
+  </si>
+  <si>
+    <t>견고함</t>
+  </si>
+  <si>
+    <t>잠 16:6</t>
+  </si>
+  <si>
+    <t>죄악을 피할 능력</t>
+  </si>
+  <si>
+    <t>눅 1:50</t>
+  </si>
+  <si>
+    <t>하나님의 자비</t>
+  </si>
+  <si>
+    <t>행 10:35</t>
+  </si>
+  <si>
+    <t>하나님의 인정하심</t>
+  </si>
+  <si>
+    <t>seq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subseq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int(8)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8074,8 +8320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B438DAE-6F36-41E3-B6E7-010F6023C9BC}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8452,4 +8698,620 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B9BA6-85D1-4B72-A95E-1D25C735695A}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="37.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>38</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>